<commit_message>
requirement updated in excel
</commit_message>
<xml_diff>
--- a/requirements.xlsx
+++ b/requirements.xlsx
@@ -5,16 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\project2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\figma\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{953AF9F7-E6A7-4837-B09A-62166342DE63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1473A3A3-BE28-445F-A099-6AE8942A950D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{9B9954AE-27A8-4982-954F-66D15F794264}"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="21600" windowHeight="12645" xr2:uid="{9B9954AE-27A8-4982-954F-66D15F794264}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Daily Tasks" sheetId="2" r:id="rId2"/>
+    <sheet name="Figma Queries" sheetId="1" r:id="rId1"/>
+    <sheet name="Daily Tasks" sheetId="2" state="hidden" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -320,6 +320,14 @@
   </cellStyles>
   <dxfs count="4">
     <dxf>
+      <numFmt numFmtId="164" formatCode="[$]dd/mmm/yy;@" x16r2:formatCode16="[$-en-PK,1]dd/mmm/yy;@"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <font>
         <color rgb="FF9C0006"/>
       </font>
@@ -338,14 +346,6 @@
           <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="[$]dd/mmm/yy;@" x16r2:formatCode16="[$-en-PK,1]dd/mmm/yy;@"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -371,8 +371,8 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F59570DF-D901-4A01-87C9-E40F604C6CC2}" name="Table1" displayName="Table1" ref="A1:D25" totalsRowShown="0">
   <autoFilter ref="A1:D25" xr:uid="{F59570DF-D901-4A01-87C9-E40F604C6CC2}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{5009B7BE-FA3E-42D1-A3A7-ADFDBE142F67}" name="Day" dataDxfId="3"/>
-    <tableColumn id="4" xr3:uid="{840CBA56-9D8F-4DAC-8324-B50671BAC3EA}" name="Date" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{5009B7BE-FA3E-42D1-A3A7-ADFDBE142F67}" name="Day" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{840CBA56-9D8F-4DAC-8324-B50671BAC3EA}" name="Date" dataDxfId="0"/>
     <tableColumn id="2" xr3:uid="{92688EF5-C27C-455B-BB57-170276A463AF}" name="Task Completed"/>
     <tableColumn id="3" xr3:uid="{E7D883C0-BDB9-40F9-863F-399D7734E280}" name="Remarks"/>
   </tableColumns>
@@ -680,7 +680,7 @@
   <dimension ref="A1:K28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1212,10 +1212,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A4:A9 A2 A11:A16 A18:A23 A25">
-    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="Sun">
+    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="Sun">
       <formula>NOT(ISERROR(SEARCH("Sun",A2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="2" operator="containsText" text="Sat">
+    <cfRule type="containsText" dxfId="2" priority="2" operator="containsText" text="Sat">
       <formula>NOT(ISERROR(SEARCH("Sat",A2)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>